<commit_message>
add iphone icons and loading view
</commit_message>
<xml_diff>
--- a/test/test plan.xlsx
+++ b/test/test plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="0" windowWidth="24140" windowHeight="15880" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24540" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t>app icon</t>
   </si>
@@ -198,9 +198,6 @@
     <t>推荐活动</t>
   </si>
   <si>
-    <t>每一项没填，点击“发布活动”，查看报错“请填写活动详情，吸引更多的同学来报名参加”</t>
-  </si>
-  <si>
     <t>输入每项内容可点击预览查看</t>
   </si>
   <si>
@@ -322,6 +319,27 @@
   </si>
   <si>
     <t>添加活动美图，一，用户自己上传；二，用户不上传随机使用给出的默认图片</t>
+  </si>
+  <si>
+    <t>内容填写完整，点击注册button，注册成功</t>
+  </si>
+  <si>
+    <t>一般情况</t>
+  </si>
+  <si>
+    <t>Functional Testing</t>
+  </si>
+  <si>
+    <t>在每一项空着的情况下，点击“发布活动”，查看报错“请填写活动详情，吸引更多的同学来报名参加”</t>
+  </si>
+  <si>
+    <t>通过人人登录用户</t>
+  </si>
+  <si>
+    <t>正常注册用户</t>
+  </si>
+  <si>
+    <t>分享勾中状态需要授权</t>
   </si>
 </sst>
 </file>
@@ -444,7 +462,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="16">
+  <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -461,8 +479,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -470,12 +492,15 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -485,7 +510,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="16">
+  <cellStyles count="20">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -493,6 +518,8 @@
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -500,6 +527,8 @@
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
@@ -830,17 +859,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17.1640625" customWidth="1"/>
-    <col min="2" max="2" width="5.1640625" customWidth="1"/>
-    <col min="3" max="3" width="94.83203125" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="107.1640625" customWidth="1"/>
     <col min="4" max="4" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -881,19 +910,19 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="17">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="7"/>
+      <c r="B4" s="6"/>
       <c r="C4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="9"/>
+      <c r="B5" s="7"/>
       <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
@@ -901,391 +930,411 @@
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:6" ht="17">
-      <c r="A6" s="6"/>
-      <c r="B6" s="9"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="7"/>
       <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="17">
-      <c r="A7" s="6"/>
-      <c r="B7" s="9"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="7"/>
       <c r="C7" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="17">
+      <c r="A8" s="10"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17">
-      <c r="A8" s="6"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
     <row r="9" spans="1:6" ht="17">
-      <c r="A9" s="6"/>
-      <c r="B9" s="9"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="7"/>
       <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="17">
-      <c r="A10" s="6"/>
-      <c r="B10" s="9"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="7"/>
       <c r="C10" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="17">
-      <c r="A11" s="6"/>
-      <c r="B11" s="9"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="7"/>
       <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="17">
-      <c r="A12" s="6"/>
-      <c r="B12" s="9"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="7"/>
       <c r="C12" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="17">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="9"/>
+      <c r="B13" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="C13" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="17">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="17">
-      <c r="A14" s="6"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="1" t="s">
+    <row r="15" spans="1:6" ht="17">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="17">
-      <c r="A15" s="6"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="1" t="s">
+    <row r="16" spans="1:6" ht="17">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="17">
-      <c r="A16" s="6"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="1" t="s">
+    <row r="17" spans="1:3" ht="17">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="17">
-      <c r="A17" s="6"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="1" t="s">
+    <row r="18" spans="1:3" ht="17">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17">
-      <c r="A18" s="6"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="1" t="s">
+    <row r="19" spans="1:3" ht="17">
+      <c r="A19" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17">
-      <c r="A19" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="1" t="s">
+    <row r="20" spans="1:3" ht="17">
+      <c r="A20" s="10"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17">
-      <c r="A20" s="6"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="1" t="s">
+    <row r="21" spans="1:3" ht="17">
+      <c r="A21" s="10"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="17">
-      <c r="A21" s="6"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="1" t="s">
+    <row r="22" spans="1:3" ht="17">
+      <c r="A22" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="7"/>
+      <c r="C22" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="17">
-      <c r="A22" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="1" t="s">
+    <row r="23" spans="1:3" ht="17">
+      <c r="A23" s="10"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="17">
-      <c r="A23" s="6"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="1" t="s">
+    <row r="24" spans="1:3" ht="17">
+      <c r="A24" s="10"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="17">
-      <c r="A24" s="6"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="1" t="s">
+    <row r="25" spans="1:3" ht="17">
+      <c r="A25" s="10"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="17">
-      <c r="A25" s="6"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="1" t="s">
+    <row r="26" spans="1:3" ht="17">
+      <c r="A26" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="17">
-      <c r="A26" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="1" t="s">
+    <row r="27" spans="1:3" ht="17">
+      <c r="A27" s="10"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="17">
-      <c r="A27" s="6"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="1" t="s">
+    <row r="28" spans="1:3" ht="17">
+      <c r="A28" s="10"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="17">
-      <c r="A28" s="6"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="1" t="s">
+    <row r="29" spans="1:3" ht="17">
+      <c r="A29" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="7"/>
+      <c r="C29" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="17">
-      <c r="A29" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="1" t="s">
+    <row r="30" spans="1:3" ht="17">
+      <c r="A30" s="10"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="17">
-      <c r="A30" s="6"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="1" t="s">
+    <row r="31" spans="1:3" ht="18" customHeight="1">
+      <c r="A31" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="7"/>
+      <c r="C31" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="18" customHeight="1">
-      <c r="A31" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="1" t="s">
+    <row r="32" spans="1:3" ht="17">
+      <c r="A32" s="10"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="17">
+      <c r="A33" s="10"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="17">
-      <c r="A32" s="6"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="1" t="s">
+    <row r="34" spans="1:3" ht="17">
+      <c r="A34" s="10"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="17">
-      <c r="A33" s="6"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="17">
-      <c r="A34" s="6"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
     <row r="35" spans="1:3" ht="17">
-      <c r="A35" s="6"/>
-      <c r="B35" s="9"/>
+      <c r="A35" s="10"/>
+      <c r="B35" s="7"/>
       <c r="C35" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="17">
-      <c r="A36" s="6"/>
-      <c r="B36" s="9"/>
+      <c r="A36" s="10"/>
+      <c r="B36" s="9" t="s">
+        <v>76</v>
+      </c>
       <c r="C36" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="17">
+      <c r="A37" s="10"/>
+      <c r="B37" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="17">
+      <c r="A38" s="6" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="18">
-      <c r="A37" s="6" t="s">
+      <c r="B38" s="7"/>
+      <c r="C38" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="18">
+      <c r="A39" s="6"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="B37" s="9"/>
-      <c r="C37" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="17">
-      <c r="A38" s="6"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="17">
-      <c r="A39" s="6"/>
-      <c r="B39" s="9"/>
-      <c r="C39" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="17">
       <c r="A40" s="6"/>
-      <c r="B40" s="9"/>
+      <c r="B40" s="7"/>
       <c r="C40" s="1" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="17">
       <c r="A41" s="6"/>
-      <c r="B41" s="9"/>
+      <c r="B41" s="7"/>
       <c r="C41" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="18">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="17">
       <c r="A42" s="6"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="2" t="s">
-        <v>50</v>
+      <c r="B42" s="7"/>
+      <c r="C42" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="17">
       <c r="A43" s="6"/>
-      <c r="B43" s="9"/>
+      <c r="B43" s="7"/>
       <c r="C43" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="17">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="18">
       <c r="A44" s="6"/>
-      <c r="B44" s="9"/>
-      <c r="C44" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="18">
+      <c r="B44" s="7"/>
+      <c r="C44" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="17">
       <c r="A45" s="6"/>
-      <c r="B45" s="9"/>
-      <c r="C45" s="2" t="s">
-        <v>53</v>
+      <c r="B45" s="7"/>
+      <c r="C45" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="17">
       <c r="A46" s="6"/>
-      <c r="B46" s="9"/>
+      <c r="B46" s="7"/>
       <c r="C46" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="17">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="18">
       <c r="A47" s="6"/>
-      <c r="B47" s="9"/>
-      <c r="C47" s="1" t="s">
-        <v>54</v>
+      <c r="B47" s="7"/>
+      <c r="C47" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="17">
       <c r="A48" s="6"/>
-      <c r="B48" s="9"/>
+      <c r="B48" s="7"/>
       <c r="C48" s="1" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="18" customHeight="1">
       <c r="A49" s="6"/>
-      <c r="B49" s="9"/>
+      <c r="B49" s="7"/>
       <c r="C49" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="18">
-      <c r="A50" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="B50" s="10"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="17">
+      <c r="A50" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B50" s="7"/>
       <c r="C50" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="18">
-      <c r="A51" s="8"/>
-      <c r="B51" s="10"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="17">
+      <c r="A51" s="11"/>
+      <c r="B51" s="7"/>
       <c r="C51" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="18">
       <c r="A52" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B52" s="8"/>
+      <c r="C52" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="18" customHeight="1">
+      <c r="A53" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B53" s="8"/>
+      <c r="C53" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="18">
+      <c r="A54" s="11"/>
+      <c r="B54" s="8"/>
+      <c r="C54" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="17">
+      <c r="B55" s="1"/>
+      <c r="C55" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="18">
+      <c r="B56" s="8"/>
+      <c r="C56" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B52" s="10"/>
-      <c r="C52" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="18" customHeight="1">
-      <c r="A53" s="8" t="s">
+    </row>
+    <row r="57" spans="1:3" ht="18">
+      <c r="B57" s="8"/>
+      <c r="C57" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="18">
-      <c r="A54" s="8"/>
-      <c r="B54" s="10"/>
-      <c r="C54" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="18">
-      <c r="B55" s="10"/>
-      <c r="C55" s="1" t="s">
+    </row>
+    <row r="58" spans="1:3" ht="17">
+      <c r="C58" s="1" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="17">
-      <c r="C56" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A31:A36"/>
-    <mergeCell ref="A37:A49"/>
     <mergeCell ref="A5:A12"/>
     <mergeCell ref="A13:A18"/>
     <mergeCell ref="A19:A21"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="A50:A51"/>
     <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A37"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>